<commit_message>
Updates for reviewer comments
Added supplemental data (Supp Fig1 and Supp Fig5) and re-plotted OMX data in figure 6. Re-named other supplemental figures to reflect new ordering.
</commit_message>
<xml_diff>
--- a/Figure6/Fig6 data.xlsx
+++ b/Figure6/Fig6 data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rcsegura/Desktop/PP4_github/Figure6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234F885B-C98A-4F47-8736-D54C3582DD7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6A596D-6630-464F-80F7-0176857F53B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{53979465-41B2-FF48-B22D-C4264CD05F24}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{53979465-41B2-FF48-B22D-C4264CD05F24}"/>
   </bookViews>
   <sheets>
     <sheet name="Fig6E, F, G" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="325">
   <si>
     <t>File Name</t>
   </si>
@@ -987,12 +987,6 @@
     <t>ns</t>
   </si>
   <si>
-    <t>Exact Wilcoxon Rank-Sum Test</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Mann-Whitney U Test</t>
   </si>
   <si>
@@ -1008,34 +1002,13 @@
     <t>6E</t>
   </si>
   <si>
-    <t>control enrichment</t>
-  </si>
-  <si>
-    <t>experimental enrichment</t>
-  </si>
-  <si>
-    <t>Daughter</t>
-  </si>
-  <si>
-    <t>Mother</t>
-  </si>
-  <si>
     <t>****</t>
-  </si>
-  <si>
-    <t>Symmetric</t>
-  </si>
-  <si>
-    <t>None</t>
   </si>
   <si>
     <t>6F</t>
   </si>
   <si>
     <t>Chi^2 goodness of fit</t>
-  </si>
-  <si>
-    <t>6G</t>
   </si>
 </sst>
 </file>
@@ -1927,7 +1900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53711834-DBD5-DF48-B5BD-7DDE4287E173}">
   <dimension ref="A1:DG186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CF1" workbookViewId="0">
+    <sheetView topLeftCell="CF1" workbookViewId="0">
       <selection activeCell="CM1" sqref="CM1"/>
     </sheetView>
   </sheetViews>
@@ -47176,17 +47149,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6F2854-4595-8F47-BBE2-1725FEDBDECF}">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C1" t="s">
         <v>298</v>
@@ -47237,12 +47210,12 @@
         <v>312</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C2" t="s">
         <v>151</v>
@@ -47251,54 +47224,54 @@
         <v>112</v>
       </c>
       <c r="E2" t="s">
-        <v>208</v>
+        <v>178</v>
       </c>
       <c r="F2" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="G2" t="s">
         <v>314</v>
       </c>
       <c r="H2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I2">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="J2">
-        <v>-0.23653744183040301</v>
+        <v>-0.202898991811512</v>
       </c>
       <c r="K2">
-        <v>-0.212611430826219</v>
+        <v>7.8031729607426201E-2</v>
       </c>
       <c r="L2">
-        <v>0.185705294403855</v>
+        <v>0.16937536243850701</v>
       </c>
       <c r="M2">
-        <v>0.12528014049693401</v>
+        <v>0.571894183769874</v>
       </c>
       <c r="N2">
-        <v>-0.31813581877243302</v>
-      </c>
-      <c r="O2">
-        <v>15</v>
+        <v>54</v>
+      </c>
+      <c r="O2" t="s">
+        <v>315</v>
       </c>
       <c r="P2" t="s">
         <v>315</v>
       </c>
       <c r="Q2" s="5">
-        <v>0.75476799999999999</v>
+        <v>0.33834199999999998</v>
       </c>
       <c r="R2" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C3" t="s">
         <v>151</v>
@@ -47307,7 +47280,7 @@
         <v>261</v>
       </c>
       <c r="E3" t="s">
-        <v>208</v>
+        <v>178</v>
       </c>
       <c r="F3" t="s">
         <v>317</v>
@@ -47316,25 +47289,25 @@
         <v>314</v>
       </c>
       <c r="H3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I3">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="J3">
-        <v>-0.23653744183040301</v>
+        <v>-0.202898991811512</v>
       </c>
       <c r="K3">
-        <v>-0.48679839304449701</v>
+        <v>-0.43678632018337499</v>
       </c>
       <c r="L3">
-        <v>0.185705294403855</v>
+        <v>0.16937536243850701</v>
       </c>
       <c r="M3">
-        <v>0.34911121273669299</v>
+        <v>0.26766998940028702</v>
       </c>
       <c r="N3">
-        <v>1.64316767251549</v>
+        <v>89</v>
       </c>
       <c r="O3" t="s">
         <v>315</v>
@@ -47343,18 +47316,18 @@
         <v>315</v>
       </c>
       <c r="Q3" s="5">
-        <v>0.10034800000000001</v>
+        <v>5.9560699999999999E-3</v>
       </c>
       <c r="R3" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C4" t="s">
         <v>151</v>
@@ -47363,54 +47336,54 @@
         <v>112</v>
       </c>
       <c r="E4" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="F4" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="G4" t="s">
         <v>314</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="I4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J4">
-        <v>-0.10198364175484</v>
+        <v>-0.12918857026252001</v>
       </c>
       <c r="K4">
-        <v>0.53475669600315401</v>
+        <v>8.003239385633E-2</v>
       </c>
       <c r="L4">
-        <v>3.5024624023060301E-2</v>
+        <v>0.56037496709263102</v>
       </c>
       <c r="M4">
-        <v>0.70872271987449098</v>
-      </c>
-      <c r="N4" t="s">
-        <v>318</v>
-      </c>
-      <c r="O4" t="s">
-        <v>318</v>
+        <v>0.36621757498281199</v>
+      </c>
+      <c r="N4">
+        <v>-0.962148161481158</v>
+      </c>
+      <c r="O4">
+        <v>18</v>
       </c>
       <c r="P4" t="s">
-        <v>318</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>318</v>
+        <v>315</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0.34872300000000001</v>
       </c>
       <c r="R4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C5" t="s">
         <v>151</v>
@@ -47419,54 +47392,54 @@
         <v>261</v>
       </c>
       <c r="E5" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="F5" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="G5" t="s">
         <v>314</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="I5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J5">
-        <v>-0.10198364175484</v>
+        <v>-0.12918857026252001</v>
       </c>
       <c r="K5">
-        <v>-0.40552877464517301</v>
+        <v>-0.39640492036407199</v>
       </c>
       <c r="L5">
-        <v>3.5024624023060301E-2</v>
+        <v>0.56037496709263102</v>
       </c>
       <c r="M5">
-        <v>0.224222406452913</v>
-      </c>
-      <c r="N5" t="s">
-        <v>318</v>
-      </c>
-      <c r="O5" t="s">
-        <v>318</v>
+        <v>0.21352981105697599</v>
+      </c>
+      <c r="N5">
+        <v>1.34728753656157</v>
+      </c>
+      <c r="O5">
+        <v>18</v>
       </c>
       <c r="P5" t="s">
-        <v>318</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>318</v>
+        <v>315</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>0.194604</v>
       </c>
       <c r="R5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C6" t="s">
         <v>151</v>
@@ -47475,7 +47448,7 @@
         <v>112</v>
       </c>
       <c r="E6" t="s">
-        <v>159</v>
+        <v>189</v>
       </c>
       <c r="F6" t="s">
         <v>313</v>
@@ -47484,45 +47457,45 @@
         <v>314</v>
       </c>
       <c r="H6">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="I6">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J6">
-        <v>-0.12918857026252001</v>
+        <v>0.142400300733528</v>
       </c>
       <c r="K6">
-        <v>8.003239385633E-2</v>
+        <v>8.2076517297887397E-2</v>
       </c>
       <c r="L6">
-        <v>0.56037496709263102</v>
+        <v>0.30982046144020597</v>
       </c>
       <c r="M6">
-        <v>0.36621757498281199</v>
+        <v>0.112472964596463</v>
       </c>
       <c r="N6">
-        <v>-0.962148161481158</v>
+        <v>0.36628893988399602</v>
       </c>
       <c r="O6">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="P6" t="s">
         <v>315</v>
       </c>
       <c r="Q6" s="5">
-        <v>0.34872300000000001</v>
+        <v>0.72497</v>
       </c>
       <c r="R6" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C7" t="s">
         <v>151</v>
@@ -47531,7 +47504,7 @@
         <v>261</v>
       </c>
       <c r="E7" t="s">
-        <v>159</v>
+        <v>189</v>
       </c>
       <c r="F7" t="s">
         <v>313</v>
@@ -47540,45 +47513,45 @@
         <v>314</v>
       </c>
       <c r="H7">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="I7">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J7">
-        <v>-0.12918857026252001</v>
+        <v>0.142400300733528</v>
       </c>
       <c r="K7">
-        <v>-0.39640492036407199</v>
+        <v>-0.35656857510624101</v>
       </c>
       <c r="L7">
-        <v>0.56037496709263102</v>
+        <v>0.30982046144020597</v>
       </c>
       <c r="M7">
-        <v>0.21352981105697599</v>
+        <v>0.52569063436280405</v>
       </c>
       <c r="N7">
-        <v>1.34728753656157</v>
+        <v>1.82847481945831</v>
       </c>
       <c r="O7">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="P7" t="s">
         <v>315</v>
       </c>
       <c r="Q7" s="5">
-        <v>0.194604</v>
+        <v>0.104882</v>
       </c>
       <c r="R7" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C8" t="s">
         <v>151</v>
@@ -47587,54 +47560,54 @@
         <v>112</v>
       </c>
       <c r="E8" t="s">
-        <v>189</v>
+        <v>113</v>
       </c>
       <c r="F8" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="G8" t="s">
         <v>314</v>
       </c>
       <c r="H8">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="I8">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="J8">
-        <v>0.142400300733528</v>
+        <v>0.66310530133267898</v>
       </c>
       <c r="K8">
-        <v>8.2076517297887397E-2</v>
+        <v>9.8337771609422198E-3</v>
       </c>
       <c r="L8">
-        <v>0.30982046144020597</v>
+        <v>0.61522415496984595</v>
       </c>
       <c r="M8">
-        <v>0.112472964596463</v>
+        <v>0.75754403999076203</v>
       </c>
       <c r="N8">
-        <v>0.36628893988399602</v>
-      </c>
-      <c r="O8">
-        <v>7</v>
+        <v>450</v>
+      </c>
+      <c r="O8" t="s">
+        <v>315</v>
       </c>
       <c r="P8" t="s">
         <v>315</v>
       </c>
       <c r="Q8" s="5">
-        <v>0.72497</v>
+        <v>6.24846E-3</v>
       </c>
       <c r="R8" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C9" t="s">
         <v>151</v>
@@ -47643,815 +47616,160 @@
         <v>261</v>
       </c>
       <c r="E9" t="s">
-        <v>189</v>
+        <v>113</v>
       </c>
       <c r="F9" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="G9" t="s">
         <v>314</v>
       </c>
       <c r="H9">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="I9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J9">
-        <v>0.142400300733528</v>
+        <v>0.66310530133267898</v>
       </c>
       <c r="K9">
-        <v>-0.35656857510624101</v>
+        <v>3.9064440207189098E-2</v>
       </c>
       <c r="L9">
-        <v>0.30982046144020597</v>
+        <v>0.61522415496984595</v>
       </c>
       <c r="M9">
-        <v>0.52569063436280405</v>
+        <v>0.62439886534260902</v>
       </c>
       <c r="N9">
-        <v>1.82847481945831</v>
-      </c>
-      <c r="O9">
-        <v>8</v>
+        <v>129</v>
+      </c>
+      <c r="O9" t="s">
+        <v>315</v>
       </c>
       <c r="P9" t="s">
         <v>315</v>
       </c>
       <c r="Q9" s="5">
-        <v>0.104882</v>
+        <v>2.89535E-2</v>
       </c>
       <c r="R9" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q10" s="5"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>320</v>
+      </c>
+      <c r="C12" t="s">
+        <v>298</v>
+      </c>
+      <c r="D12" t="s">
+        <v>299</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>300</v>
+      </c>
+      <c r="G12" t="s">
+        <v>302</v>
+      </c>
+      <c r="H12" t="s">
+        <v>303</v>
+      </c>
+      <c r="I12" t="s">
+        <v>308</v>
+      </c>
+      <c r="J12" t="s">
+        <v>309</v>
+      </c>
+      <c r="K12" t="s">
+        <v>311</v>
+      </c>
+      <c r="L12" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" t="s">
         <v>323</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C13" t="s">
         <v>151</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D13" t="s">
         <v>112</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E13" t="s">
         <v>113</v>
       </c>
-      <c r="F10" t="s">
-        <v>319</v>
-      </c>
-      <c r="G10" t="s">
-        <v>314</v>
-      </c>
-      <c r="H10">
+      <c r="F13" t="s">
+        <v>324</v>
+      </c>
+      <c r="G13">
         <v>17</v>
       </c>
-      <c r="I10">
+      <c r="H13">
         <v>36</v>
       </c>
-      <c r="J10">
-        <v>0.66310530133267898</v>
-      </c>
-      <c r="K10">
-        <v>9.8337771609422198E-3</v>
-      </c>
-      <c r="L10">
-        <v>0.61522415496984595</v>
-      </c>
-      <c r="M10">
-        <v>0.75754403999076203</v>
-      </c>
-      <c r="N10">
-        <v>450</v>
-      </c>
-      <c r="O10" t="s">
-        <v>315</v>
-      </c>
-      <c r="P10" t="s">
-        <v>315</v>
-      </c>
-      <c r="Q10" s="5">
-        <v>6.24846E-3</v>
-      </c>
-      <c r="R10" t="s">
-        <v>320</v>
+      <c r="I13">
+        <v>1819999999973</v>
+      </c>
+      <c r="J13">
+        <v>3</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" t="s">
+        <v>322</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B14" t="s">
         <v>323</v>
-      </c>
-      <c r="C11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D11" t="s">
-        <v>261</v>
-      </c>
-      <c r="E11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F11" t="s">
-        <v>319</v>
-      </c>
-      <c r="G11" t="s">
-        <v>314</v>
-      </c>
-      <c r="H11">
-        <v>17</v>
-      </c>
-      <c r="I11">
-        <v>10</v>
-      </c>
-      <c r="J11">
-        <v>0.66310530133267898</v>
-      </c>
-      <c r="K11">
-        <v>3.9064440207189098E-2</v>
-      </c>
-      <c r="L11">
-        <v>0.61522415496984595</v>
-      </c>
-      <c r="M11">
-        <v>0.62439886534260902</v>
-      </c>
-      <c r="N11">
-        <v>129</v>
-      </c>
-      <c r="O11" t="s">
-        <v>315</v>
-      </c>
-      <c r="P11" t="s">
-        <v>315</v>
-      </c>
-      <c r="Q11" s="5">
-        <v>2.89535E-2</v>
-      </c>
-      <c r="R11" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>322</v>
-      </c>
-      <c r="C13" t="s">
-        <v>298</v>
-      </c>
-      <c r="D13" t="s">
-        <v>324</v>
-      </c>
-      <c r="E13" t="s">
-        <v>299</v>
-      </c>
-      <c r="F13" t="s">
-        <v>325</v>
-      </c>
-      <c r="G13" t="s">
-        <v>3</v>
-      </c>
-      <c r="H13" t="s">
-        <v>300</v>
-      </c>
-      <c r="I13" t="s">
-        <v>301</v>
-      </c>
-      <c r="J13" t="s">
-        <v>302</v>
-      </c>
-      <c r="K13" t="s">
-        <v>303</v>
-      </c>
-      <c r="L13" t="s">
-        <v>304</v>
-      </c>
-      <c r="M13" t="s">
-        <v>305</v>
-      </c>
-      <c r="N13" t="s">
-        <v>306</v>
-      </c>
-      <c r="O13" t="s">
-        <v>307</v>
-      </c>
-      <c r="P13" t="s">
-        <v>308</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>309</v>
-      </c>
-      <c r="R13" t="s">
-        <v>310</v>
-      </c>
-      <c r="S13" t="s">
-        <v>311</v>
-      </c>
-      <c r="T13" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="B14" t="s">
-        <v>331</v>
       </c>
       <c r="C14" t="s">
         <v>151</v>
       </c>
       <c r="D14" t="s">
-        <v>326</v>
+        <v>261</v>
       </c>
       <c r="E14" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F14" t="s">
-        <v>326</v>
-      </c>
-      <c r="G14" t="s">
-        <v>113</v>
-      </c>
-      <c r="H14" t="s">
-        <v>319</v>
-      </c>
-      <c r="I14" t="s">
-        <v>314</v>
+        <v>324</v>
+      </c>
+      <c r="G14">
+        <v>17</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="I14">
+        <v>169999999995</v>
       </c>
       <c r="J14">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="K14">
-        <v>18</v>
-      </c>
-      <c r="L14">
-        <v>0.66310530133267898</v>
-      </c>
-      <c r="M14">
-        <v>0.509039434186777</v>
-      </c>
-      <c r="N14">
-        <v>0.61522415496984595</v>
-      </c>
-      <c r="O14">
-        <v>0.30772215071361902</v>
-      </c>
-      <c r="P14">
-        <v>163</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>315</v>
-      </c>
-      <c r="R14" t="s">
-        <v>315</v>
-      </c>
-      <c r="S14" s="5">
-        <v>0.75386500000000001</v>
-      </c>
-      <c r="T14" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>331</v>
-      </c>
-      <c r="C15" t="s">
-        <v>151</v>
-      </c>
-      <c r="D15" t="s">
-        <v>326</v>
-      </c>
-      <c r="E15" t="s">
-        <v>112</v>
-      </c>
-      <c r="F15" t="s">
-        <v>327</v>
-      </c>
-      <c r="G15" t="s">
-        <v>113</v>
-      </c>
-      <c r="H15" t="s">
-        <v>319</v>
-      </c>
-      <c r="I15" t="s">
-        <v>314</v>
-      </c>
-      <c r="J15">
-        <v>17</v>
-      </c>
-      <c r="K15">
-        <v>13</v>
-      </c>
-      <c r="L15">
-        <v>0.66310530133267898</v>
-      </c>
-      <c r="M15">
-        <v>-0.79164312589071595</v>
-      </c>
-      <c r="N15">
-        <v>0.61522415496984595</v>
-      </c>
-      <c r="O15">
-        <v>0.50696874612077103</v>
-      </c>
-      <c r="P15">
-        <v>221</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>315</v>
-      </c>
-      <c r="R15" t="s">
-        <v>315</v>
-      </c>
-      <c r="S15" s="5">
-        <v>4.1506499999999998E-6</v>
-      </c>
-      <c r="T15" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>331</v>
-      </c>
-      <c r="C16" t="s">
-        <v>151</v>
-      </c>
-      <c r="D16" t="s">
-        <v>326</v>
-      </c>
-      <c r="E16" t="s">
-        <v>112</v>
-      </c>
-      <c r="F16" t="s">
-        <v>329</v>
-      </c>
-      <c r="G16" t="s">
-        <v>113</v>
-      </c>
-      <c r="H16" t="s">
-        <v>318</v>
-      </c>
-      <c r="I16" t="s">
-        <v>314</v>
-      </c>
-      <c r="J16">
-        <v>17</v>
-      </c>
-      <c r="K16">
-        <v>2</v>
-      </c>
-      <c r="L16">
-        <v>0.66310530133267898</v>
-      </c>
-      <c r="M16">
-        <v>-3.6331394889662798E-2</v>
-      </c>
-      <c r="N16">
-        <v>0.61522415496984595</v>
-      </c>
-      <c r="O16">
-        <v>6.97913843284452E-3</v>
-      </c>
-      <c r="P16" t="s">
-        <v>318</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>318</v>
-      </c>
-      <c r="R16" t="s">
-        <v>318</v>
-      </c>
-      <c r="S16" t="s">
-        <v>318</v>
-      </c>
-      <c r="T16" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>331</v>
-      </c>
-      <c r="C17" t="s">
-        <v>151</v>
-      </c>
-      <c r="D17" t="s">
-        <v>326</v>
-      </c>
-      <c r="E17" t="s">
-        <v>112</v>
-      </c>
-      <c r="F17" t="s">
-        <v>330</v>
-      </c>
-      <c r="G17" t="s">
-        <v>113</v>
-      </c>
-      <c r="H17" t="s">
-        <v>317</v>
-      </c>
-      <c r="I17" t="s">
-        <v>314</v>
-      </c>
-      <c r="J17">
-        <v>17</v>
-      </c>
-      <c r="K17">
-        <v>3</v>
-      </c>
-      <c r="L17">
-        <v>0.66310530133267898</v>
-      </c>
-      <c r="M17">
-        <v>0.51844319626352198</v>
-      </c>
-      <c r="N17">
-        <v>0.61522415496984595</v>
-      </c>
-      <c r="O17">
-        <v>0.94200417919886503</v>
-      </c>
-      <c r="P17">
-        <v>0.68803296123245195</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>315</v>
-      </c>
-      <c r="R17" t="s">
-        <v>315</v>
-      </c>
-      <c r="S17" s="5">
-        <v>0.49143199999999998</v>
-      </c>
-      <c r="T17" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>331</v>
-      </c>
-      <c r="C18" t="s">
-        <v>151</v>
-      </c>
-      <c r="D18" t="s">
-        <v>326</v>
-      </c>
-      <c r="E18" t="s">
-        <v>261</v>
-      </c>
-      <c r="F18" t="s">
-        <v>326</v>
-      </c>
-      <c r="G18" t="s">
-        <v>113</v>
-      </c>
-      <c r="H18" t="s">
-        <v>317</v>
-      </c>
-      <c r="I18" t="s">
-        <v>314</v>
-      </c>
-      <c r="J18">
-        <v>17</v>
-      </c>
-      <c r="K18">
-        <v>5</v>
-      </c>
-      <c r="L18">
-        <v>0.66310530133267898</v>
-      </c>
-      <c r="M18">
-        <v>0.48171450804446198</v>
-      </c>
-      <c r="N18">
-        <v>0.61522415496984595</v>
-      </c>
-      <c r="O18">
-        <v>9.7263836042704596E-2</v>
-      </c>
-      <c r="P18">
-        <v>0.117519112011534</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>315</v>
-      </c>
-      <c r="R18" t="s">
-        <v>315</v>
-      </c>
-      <c r="S18" s="5">
-        <v>0.90644899999999995</v>
-      </c>
-      <c r="T18" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>331</v>
-      </c>
-      <c r="C19" t="s">
-        <v>151</v>
-      </c>
-      <c r="D19" t="s">
-        <v>326</v>
-      </c>
-      <c r="E19" t="s">
-        <v>261</v>
-      </c>
-      <c r="F19" t="s">
-        <v>327</v>
-      </c>
-      <c r="G19" t="s">
-        <v>113</v>
-      </c>
-      <c r="H19" t="s">
-        <v>317</v>
-      </c>
-      <c r="I19" t="s">
-        <v>314</v>
-      </c>
-      <c r="J19">
-        <v>17</v>
-      </c>
-      <c r="K19">
-        <v>4</v>
-      </c>
-      <c r="L19">
-        <v>0.66310530133267898</v>
-      </c>
-      <c r="M19">
-        <v>-0.50581316059890802</v>
-      </c>
-      <c r="N19">
-        <v>0.61522415496984595</v>
-      </c>
-      <c r="O19">
-        <v>0.65894468069836498</v>
-      </c>
-      <c r="P19">
-        <v>3.0451153135353102</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>315</v>
-      </c>
-      <c r="R19" t="s">
-        <v>315</v>
-      </c>
-      <c r="S19" s="5">
-        <v>2.32591E-3</v>
-      </c>
-      <c r="T19" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>6</v>
-      </c>
-      <c r="B20" t="s">
-        <v>331</v>
-      </c>
-      <c r="C20" t="s">
-        <v>151</v>
-      </c>
-      <c r="D20" t="s">
-        <v>326</v>
-      </c>
-      <c r="E20" t="s">
-        <v>261</v>
-      </c>
-      <c r="F20" t="s">
-        <v>329</v>
-      </c>
-      <c r="G20" t="s">
-        <v>113</v>
-      </c>
-      <c r="H20" t="s">
-        <v>318</v>
-      </c>
-      <c r="I20" t="s">
-        <v>314</v>
-      </c>
-      <c r="J20">
-        <v>17</v>
-      </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20">
-        <v>0.66310530133267898</v>
-      </c>
-      <c r="M20">
-        <v>5.32450424521281E-3</v>
-      </c>
-      <c r="N20">
-        <v>0.61522415496984595</v>
-      </c>
-      <c r="P20" t="s">
-        <v>318</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>318</v>
-      </c>
-      <c r="R20" t="s">
-        <v>318</v>
-      </c>
-      <c r="S20" t="s">
-        <v>318</v>
-      </c>
-      <c r="T20" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>7</v>
-      </c>
-      <c r="B21" t="s">
-        <v>331</v>
-      </c>
-      <c r="C21" t="s">
-        <v>151</v>
-      </c>
-      <c r="D21" t="s">
-        <v>326</v>
-      </c>
-      <c r="E21" t="s">
-        <v>261</v>
-      </c>
-      <c r="F21" t="s">
-        <v>330</v>
-      </c>
-      <c r="G21" t="s">
-        <v>113</v>
-      </c>
-      <c r="H21" t="s">
-        <v>318</v>
-      </c>
-      <c r="I21" t="s">
-        <v>314</v>
-      </c>
-      <c r="J21">
-        <v>17</v>
-      </c>
-      <c r="K21">
         <v>0</v>
       </c>
-      <c r="L21">
-        <v>0.66310530133267898</v>
-      </c>
-      <c r="N21">
-        <v>0.61522415496984595</v>
-      </c>
-      <c r="P21" t="s">
-        <v>318</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>318</v>
-      </c>
-      <c r="R21" t="s">
-        <v>318</v>
-      </c>
-      <c r="S21" t="s">
-        <v>318</v>
-      </c>
-      <c r="T21" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
+      <c r="L14" t="s">
         <v>322</v>
-      </c>
-      <c r="C23" t="s">
-        <v>298</v>
-      </c>
-      <c r="D23" t="s">
-        <v>299</v>
-      </c>
-      <c r="E23" t="s">
-        <v>3</v>
-      </c>
-      <c r="F23" t="s">
-        <v>300</v>
-      </c>
-      <c r="G23" t="s">
-        <v>302</v>
-      </c>
-      <c r="H23" t="s">
-        <v>303</v>
-      </c>
-      <c r="I23" t="s">
-        <v>308</v>
-      </c>
-      <c r="J23" t="s">
-        <v>309</v>
-      </c>
-      <c r="K23" t="s">
-        <v>311</v>
-      </c>
-      <c r="L23" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>8</v>
-      </c>
-      <c r="B24" t="s">
-        <v>333</v>
-      </c>
-      <c r="C24" t="s">
-        <v>151</v>
-      </c>
-      <c r="D24" t="s">
-        <v>112</v>
-      </c>
-      <c r="E24" t="s">
-        <v>113</v>
-      </c>
-      <c r="F24" t="s">
-        <v>332</v>
-      </c>
-      <c r="G24">
-        <v>17</v>
-      </c>
-      <c r="H24">
-        <v>36</v>
-      </c>
-      <c r="I24">
-        <v>1819999999973</v>
-      </c>
-      <c r="J24">
-        <v>3</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>9</v>
-      </c>
-      <c r="B25" t="s">
-        <v>333</v>
-      </c>
-      <c r="C25" t="s">
-        <v>151</v>
-      </c>
-      <c r="D25" t="s">
-        <v>261</v>
-      </c>
-      <c r="E25" t="s">
-        <v>113</v>
-      </c>
-      <c r="F25" t="s">
-        <v>332</v>
-      </c>
-      <c r="G25">
-        <v>17</v>
-      </c>
-      <c r="H25">
-        <v>5</v>
-      </c>
-      <c r="I25">
-        <v>169999999995</v>
-      </c>
-      <c r="J25">
-        <v>3</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25" t="s">
-        <v>328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>